<commit_message>
added insights of analysis
</commit_message>
<xml_diff>
--- a/ICC T20 World Cup Analysis.xlsx
+++ b/ICC T20 World Cup Analysis.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DS\Assignment- 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DS\Assignment- 3\t20_survey_data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A4D8F31-2EB9-4C06-ACD9-AEAD35409D0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B8650C-6162-4232-A956-8C19760E1FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
   </definedNames>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="87" r:id="rId6"/>
+    <pivotCache cacheId="14" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -656,7 +656,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -690,6 +689,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -697,7 +697,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="163">
+  <dxfs count="73">
     <dxf>
       <font>
         <name val="Abadi"/>
@@ -853,45 +853,93 @@
     </dxf>
     <dxf>
       <font>
-        <name val="Abadi"/>
-        <scheme val="none"/>
+        <color rgb="FF002060"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <name val="Abadi"/>
-        <scheme val="none"/>
+        <color rgb="FF002060"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <name val="Abadi"/>
-        <scheme val="none"/>
+        <color rgb="FF002060"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="18"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="24"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF280975"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF280975"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <sz val="14"/>
+        <color theme="0"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <sz val="14"/>
+        <color theme="0"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
     </dxf>
     <dxf>
       <fill>
@@ -915,93 +963,27 @@
       </fill>
     </dxf>
     <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
       <font>
-        <color theme="0"/>
+        <sz val="14"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <color theme="0"/>
+        <sz val="14"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF280975"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF280975"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="24"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="18"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF002060"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF002060"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF002060"/>
+        <sz val="14"/>
       </font>
     </dxf>
     <dxf>
@@ -1020,447 +1002,6 @@
       <font>
         <name val="Abadi"/>
         <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFDF49CA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFDF49CA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFDF49CA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF280975"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF280975"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="24"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="18"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF002060"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF002060"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF002060"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Abadi"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Abadi"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Abadi"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFDF49CA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFDF49CA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFDF49CA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF280975"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF280975"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="24"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="18"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF002060"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF002060"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF002060"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Abadi"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Abadi"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Abadi"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFDF49CA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFDF49CA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFDF49CA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF280975"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF280975"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="24"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="18"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF002060"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF002060"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF002060"/>
       </font>
     </dxf>
     <dxf>
@@ -1869,6 +1410,7 @@
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
+          <c:numFmt formatCode="General" sourceLinked="0"/>
           <c:spPr>
             <a:solidFill>
               <a:srgbClr val="46BDC6"/>
@@ -1904,7 +1446,7 @@
           </c:txPr>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="1"/>
           <c:showSerName val="0"/>
           <c:showPercent val="1"/>
@@ -2024,6 +1566,7 @@
             </c:spPr>
           </c:dPt>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="46BDC6"/>
@@ -2059,7 +1602,7 @@
             </c:txPr>
             <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
+            <c:showVal val="1"/>
             <c:showCatName val="1"/>
             <c:showSerName val="0"/>
             <c:showPercent val="1"/>
@@ -2124,7 +1667,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000C-34DA-4496-8689-531EC1BAAD23}"/>
+              <c16:uniqueId val="{00000009-84DE-4F2C-B841-941A4A183FE0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2565,7 +2108,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-F047-4B89-AE4A-73F516C4015E}"/>
+              <c16:uniqueId val="{00000005-CA8C-4919-B971-E6493E992887}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2880,43 +2423,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln w="12700">
-              <a:solidFill>
-                <a:schemeClr val="lt2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -3662,43 +3169,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln w="12700">
-              <a:solidFill>
-                <a:schemeClr val="lt2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -4524,43 +3995,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln w="12700">
-              <a:solidFill>
-                <a:schemeClr val="lt2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -8036,15 +7471,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>32658</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>50075</xdr:rowOff>
+      <xdr:colOff>10887</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>71846</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>87772</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>57791</xdr:rowOff>
+      <xdr:colOff>66001</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>79562</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8074,15 +7509,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>286783</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:colOff>265012</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>82731</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>171583</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>68674</xdr:rowOff>
+      <xdr:colOff>149812</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>90445</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8112,15 +7547,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:colOff>362857</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>82731</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>460829</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>68674</xdr:rowOff>
+      <xdr:colOff>341086</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>90445</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8150,15 +7585,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>21772</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>118446</xdr:rowOff>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>140217</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>10715</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>130017</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>598544</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>151789</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8188,15 +7623,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>125548</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>118446</xdr:rowOff>
+      <xdr:colOff>103777</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>140217</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>451948</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>130017</xdr:rowOff>
+      <xdr:colOff>430177</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>151789</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8233,11 +7668,11 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>275517</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>42818</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>97247</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="38" name="Team_of_Interest">
@@ -8260,7 +7695,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -8311,11 +7746,11 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>138813</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>42818</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>97247</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="39" name="Winner">
@@ -8338,7 +7773,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -8381,16 +7816,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>5923</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>31568</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>147438</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>53339</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>250371</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>131854</xdr:rowOff>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>153625</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
@@ -8426,7 +7861,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="169209" y="2404654"/>
+              <a:off x="147438" y="2371996"/>
               <a:ext cx="12773905" cy="1080000"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -8467,11 +7902,11 @@
     <xdr:to>
       <xdr:col>31</xdr:col>
       <xdr:colOff>412221</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>42818</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>97247</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="41" name="Strongest_Batting_Lineup">
@@ -8494,7 +7929,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -8545,11 +7980,11 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>398046</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>42818</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>97247</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="42" name="Strongest_Balling_Attack">
@@ -8572,7 +8007,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -8623,11 +8058,11 @@
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>255771</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>42818</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>97247</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="43" name="Top_Run_Scorer">
@@ -8650,7 +8085,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -8701,11 +8136,11 @@
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>536078</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>42818</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>97247</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="44" name="Top_Wicket_Taker">
@@ -8728,7 +8163,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -8772,15 +8207,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>280307</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>32658</xdr:rowOff>
+      <xdr:colOff>258536</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>446315</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>132944</xdr:rowOff>
+      <xdr:colOff>424544</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>154715</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
@@ -8816,7 +8251,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="12973050" y="2405744"/>
+              <a:off x="12951279" y="2373086"/>
               <a:ext cx="7481208" cy="1080000"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -8857,11 +8292,11 @@
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>82688</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>35743</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>90172</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="51" name="Key_All_Rounder">
@@ -8884,7 +8319,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -8929,7 +8364,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="zakar" refreshedDate="45449.792342361114" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="51" xr:uid="{03D5A867-01CC-46C9-86D1-AAB186174B47}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="zakar" refreshedDate="45449.822186458332" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="51" xr:uid="{03D5A867-01CC-46C9-86D1-AAB186174B47}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
@@ -9038,12 +8473,12 @@
         <s v="Mohammed Siraj"/>
         <s v="MA Starc"/>
         <s v="PJ Cummins"/>
-        <s v="bumrah"/>
         <s v="Jasprit Bumrah"/>
         <s v="JR Hazlewood"/>
         <s v="TW Hartley"/>
         <s v="Aamer Jamal"/>
         <s v="Taijul Islam"/>
+        <s v="bumrah" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Emerging_Player" numFmtId="0">
@@ -9325,7 +8760,7 @@
     <x v="2"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="4"/>
+    <x v="3"/>
     <x v="4"/>
     <x v="1"/>
   </r>
@@ -9377,7 +8812,7 @@
     <x v="3"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="5"/>
+    <x v="4"/>
     <x v="1"/>
     <x v="0"/>
   </r>
@@ -9598,7 +9033,7 @@
     <x v="6"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="5"/>
+    <x v="4"/>
     <x v="1"/>
     <x v="1"/>
   </r>
@@ -9637,7 +9072,7 @@
     <x v="4"/>
     <x v="6"/>
     <x v="5"/>
-    <x v="6"/>
+    <x v="5"/>
     <x v="5"/>
     <x v="7"/>
   </r>
@@ -9663,7 +9098,7 @@
     <x v="7"/>
     <x v="7"/>
     <x v="4"/>
-    <x v="7"/>
+    <x v="6"/>
     <x v="6"/>
     <x v="7"/>
   </r>
@@ -9689,7 +9124,7 @@
     <x v="1"/>
     <x v="7"/>
     <x v="6"/>
-    <x v="8"/>
+    <x v="7"/>
     <x v="6"/>
     <x v="3"/>
   </r>
@@ -9749,542 +9184,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7FF6719F-9D73-44D0-A275-C52D4F9B0676}" name="Age_Group/Gender" cacheId="87" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Gender">
-  <location ref="G18:H20" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="11">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item sd="0" x="1"/>
-        <item sd="0" x="0"/>
-        <item m="1" x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="8">
-        <item x="3"/>
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="5"/>
-        <item x="1"/>
-        <item m="1" x="6"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="0"/>
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Age_Group" fld="1" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B9BD4660-6BEE-4276-90A4-7D655EA47FAD}" name="PivotTable3" cacheId="87" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
-  <location ref="A4:A13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="11">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="11">
-        <item x="1"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item m="1" x="9"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="0"/>
-        <item x="3"/>
-        <item x="6"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="10"/>
-  </rowFields>
-  <rowItems count="9">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F6343D5E-15BA-4AE8-965B-F04ACCF4C37E}" name="Strongest Batting Lineup" cacheId="87" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6" rowHeaderCaption="Team">
-  <location ref="J10:K18" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="11">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="9">
-        <item x="3"/>
-        <item x="7"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item x="6"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="5"/>
-  </rowFields>
-  <rowItems count="8">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Strongest_Batting_Lineup" fld="5" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="9">
-    <chartFormat chart="4" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="3">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="4">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="5">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="6">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="7">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="8">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="9">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="10">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1E1D4E6E-1D96-430A-BB22-F0769032F7BD}" name="Winner" cacheId="87" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Team">
-  <location ref="N9:O16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="11">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="8">
-        <item x="0"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="5"/>
-        <item x="2"/>
-        <item x="6"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Winner" fld="3" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="9">
-    <chartFormat chart="5" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="5" format="3">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="5" format="4">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="5" format="5">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="5" format="6">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="5" format="7">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="5" format="8">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="5" format="9">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="5" format="10">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7EDCAE42-021E-4BE5-99A1-66D29692901B}" name="PivotTable8" cacheId="87" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Gender">
-  <location ref="G2:G3" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="11">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Total Respondants" fld="3" subtotal="count" baseField="0" baseItem="1433910992"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{53BE2CC6-82D0-4310-85DA-03654D06DEE7}" name="Gender Wise Distribution" cacheId="87" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9" rowHeaderCaption="Gender">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{53BE2CC6-82D0-4310-85DA-03654D06DEE7}" name="Gender Wise Distribution" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11" rowHeaderCaption="Gender">
   <location ref="G5:H7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -10385,15 +9285,15 @@
     </pivotField>
     <pivotField showAll="0">
       <items count="10">
-        <item x="7"/>
+        <item x="6"/>
+        <item m="1" x="8"/>
         <item x="3"/>
         <item x="4"/>
-        <item x="5"/>
         <item x="1"/>
         <item x="0"/>
         <item x="2"/>
-        <item x="8"/>
-        <item x="6"/>
+        <item x="7"/>
+        <item x="5"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -10489,8 +9389,149 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DF1C0790-5640-4024-B28D-D52689B6B629}" name="Stongest Balling Attack" cacheId="87" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9" rowHeaderCaption="Team">
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7FF6719F-9D73-44D0-A275-C52D4F9B0676}" name="Age_Group/Gender" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Gender">
+  <location ref="G18:H20" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="11">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item sd="0" x="1"/>
+        <item sd="0" x="0"/>
+        <item m="1" x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="8">
+        <item x="3"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="5"/>
+        <item x="1"/>
+        <item m="1" x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="0"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Age_Group" fld="1" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B9BD4660-6BEE-4276-90A4-7D655EA47FAD}" name="PivotTable3" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Team">
+  <location ref="A4:A13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="11">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="11">
+        <item x="1"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item m="1" x="9"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="10"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DF1C0790-5640-4024-B28D-D52689B6B629}" name="Stongest Balling Attack" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9" rowHeaderCaption="Team">
   <location ref="J22:K31" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -10687,8 +9728,190 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{27C0F334-0936-4D8B-8E95-F7671C620A6C}" name="Age Group Wise Distribution" cacheId="87" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Age Group">
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F6343D5E-15BA-4AE8-965B-F04ACCF4C37E}" name="Strongest Batting Lineup" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6" rowHeaderCaption="Team">
+  <location ref="J10:K18" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="11">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="9">
+        <item x="3"/>
+        <item x="7"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="6"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="5"/>
+  </rowFields>
+  <rowItems count="8">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Strongest_Batting_Lineup" fld="5" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="9">
+    <chartFormat chart="4" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="5">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="6">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="7">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="8">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="9">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="10">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{27C0F334-0936-4D8B-8E95-F7671C620A6C}" name="Age Group Wise Distribution" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Age Group">
   <location ref="G10:H16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -10781,15 +10004,15 @@
     </pivotField>
     <pivotField showAll="0">
       <items count="10">
-        <item x="7"/>
+        <item x="6"/>
+        <item m="1" x="8"/>
         <item x="3"/>
         <item x="4"/>
-        <item x="5"/>
         <item x="1"/>
         <item x="0"/>
         <item x="2"/>
-        <item x="8"/>
-        <item x="6"/>
+        <item x="7"/>
+        <item x="5"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -10891,8 +10114,220 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1E1D4E6E-1D96-430A-BB22-F0769032F7BD}" name="Winner" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Team">
+  <location ref="N9:O16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="11">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="8">
+        <item x="0"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="5"/>
+        <item x="2"/>
+        <item x="6"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Winner" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="9">
+    <chartFormat chart="5" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="5">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="6">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="7">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="8">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="9">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="10">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7EDCAE42-021E-4BE5-99A1-66D29692901B}" name="PivotTable8" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Gender">
+  <location ref="G2:G3" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="11">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Total Respondants" fld="3" subtotal="count" baseField="0" baseItem="1433910992"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CF22EC45-5E37-463F-B5B1-AA2AC4DD74D5}" name="PivotTable13" cacheId="87" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Gender">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CF22EC45-5E37-463F-B5B1-AA2AC4DD74D5}" name="PivotTable13" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Gender">
   <location ref="B6:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -10917,94 +10352,94 @@
     <dataField name="Total Respondants" fld="3" subtotal="count" baseField="0" baseItem="1433910992"/>
   </dataFields>
   <formats count="30">
-    <format dxfId="120">
+    <format dxfId="59">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="121">
+    <format dxfId="58">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="122">
+    <format dxfId="57">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="123">
+    <format dxfId="56">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="124">
+    <format dxfId="55">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="125">
+    <format dxfId="54">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="126">
+    <format dxfId="53">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="127">
+    <format dxfId="52">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="128">
+    <format dxfId="51">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="129">
+    <format dxfId="50">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="130">
+    <format dxfId="49">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="131">
+    <format dxfId="48">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="132">
+    <format dxfId="47">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="133">
+    <format dxfId="46">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="134">
+    <format dxfId="45">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="135">
+    <format dxfId="44">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="136">
+    <format dxfId="43">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="137">
+    <format dxfId="42">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="138">
+    <format dxfId="41">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="139">
+    <format dxfId="40">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="140">
+    <format dxfId="39">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="141">
+    <format dxfId="38">
       <pivotArea dataOnly="0" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="142">
+    <format dxfId="37">
       <pivotArea dataOnly="0" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="143">
+    <format dxfId="36">
       <pivotArea dataOnly="0" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="144">
+    <format dxfId="35">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="145">
+    <format dxfId="34">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="146">
+    <format dxfId="33">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="147">
+    <format dxfId="32">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="148">
+    <format dxfId="31">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="149">
+    <format dxfId="30">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -11145,15 +10580,15 @@
   <data>
     <tabular pivotCacheId="579991846">
       <items count="9">
-        <i x="7" s="1"/>
+        <i x="6" s="1"/>
         <i x="3" s="1"/>
         <i x="4" s="1"/>
-        <i x="5" s="1"/>
         <i x="1" s="1"/>
         <i x="0" s="1"/>
         <i x="2" s="1"/>
-        <i x="8" s="1"/>
-        <i x="6" s="1"/>
+        <i x="7" s="1"/>
+        <i x="5" s="1"/>
+        <i x="8" s="1" nd="1"/>
       </items>
     </tabular>
   </data>
@@ -11245,7 +10680,7 @@
   <slicer name="Strongest_Batting_Lineup" xr10:uid="{DAB9A7A8-B8FF-46CC-963B-7EACD3135F70}" cache="Slicer_Strongest_Batting_Lineup" caption="Strongest_Batting_Lineup" columnCount="2" style="SlicerStyleLight6" rowHeight="209550"/>
   <slicer name="Strongest_Balling_Attack" xr10:uid="{8D4FFA51-42D4-41E4-8E0A-D06752767DFD}" cache="Slicer_Strongest_Balling_Attack" caption="Strongest_Balling_Attack" columnCount="2" style="SlicerStyleLight6" rowHeight="209550"/>
   <slicer name="Top_Run_Scorer" xr10:uid="{1F2AAA9E-250C-4FF7-B058-71FC687967C3}" cache="Slicer_Top_Run_Scorer" caption="Top_Run_Scorer" columnCount="2" style="SlicerStyleLight6" rowHeight="209550"/>
-  <slicer name="Top_Wicket_Taker" xr10:uid="{3C92FC96-129C-4B7C-9C5F-CC1E8E701778}" cache="Slicer_Top_Wicket_Taker" caption="Top_Wicket_Taker" columnCount="2" style="SlicerStyleLight6" rowHeight="209550"/>
+  <slicer name="Top_Wicket_Taker" xr10:uid="{3C92FC96-129C-4B7C-9C5F-CC1E8E701778}" cache="Slicer_Top_Wicket_Taker" caption="Top_Wicket_Taker" startItem="2" columnCount="2" style="SlicerStyleLight6" rowHeight="209550"/>
   <slicer name="Emerging_Player" xr10:uid="{144CCB9B-8D1A-4A45-B96A-526645880A5E}" cache="Slicer_Emerging_Player" caption="Emerging_Player" columnCount="4" style="SlicerStyleLight6" rowHeight="209550"/>
   <slicer name="Finalists" xr10:uid="{590857C3-485A-4DA9-AA2A-D1BA808F84F2}" cache="Slicer_Finalists" caption="Finalists" columnCount="8" style="SlicerStyleLight6" rowHeight="209550"/>
   <slicer name="Key_All_Rounder" xr10:uid="{E0D05F72-46CD-433A-8F6E-FF7500EEF00D}" cache="Slicer_Key_All_Rounder" caption="Key_All_Rounder" columnCount="2" style="SlicerStyleLight6" rowHeight="209550"/>
@@ -11253,20 +10688,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{01EE1B51-9A7D-4B1A-8EB0-845421C23737}" name="Table1" displayName="Table1" ref="A1:K52" totalsRowShown="0" headerRowDxfId="162" dataDxfId="161">
-  <autoFilter ref="A1:K52" xr:uid="{01EE1B51-9A7D-4B1A-8EB0-845421C23737}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{01EE1B51-9A7D-4B1A-8EB0-845421C23737}" name="Table1" displayName="Table1" ref="A1:K52" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71">
+  <autoFilter ref="A1:K52" xr:uid="{01EE1B51-9A7D-4B1A-8EB0-845421C23737}">
+    <filterColumn colId="8">
+      <filters>
+        <filter val="bumrah"/>
+        <filter val="Jasprit Bumrah"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{75EBE216-597C-4C4A-B726-D99C39CCDB60}" name="Gender" dataDxfId="160"/>
-    <tableColumn id="2" xr3:uid="{E9F87583-4B25-409A-B140-DFEC87BF0855}" name="Age_Group" dataDxfId="159"/>
-    <tableColumn id="3" xr3:uid="{6CDA1287-CEC1-4795-8B0F-543D1C880301}" name="Team_of_Interest" dataDxfId="158"/>
-    <tableColumn id="4" xr3:uid="{22AEE1FA-C932-4088-A580-94AB0983CB55}" name="Winner" dataDxfId="157"/>
-    <tableColumn id="5" xr3:uid="{25F583BB-3320-4533-9A51-8C2F9A17EB78}" name="Finalists" dataDxfId="156"/>
-    <tableColumn id="6" xr3:uid="{A2BFDA0E-B228-4DA3-B139-0E06004025ED}" name="Strongest_Batting_Lineup" dataDxfId="155"/>
-    <tableColumn id="7" xr3:uid="{1C2F6CC1-A9AC-4C80-B2B0-CD1FF333E7E1}" name="Strongest_Balling_Attack" dataDxfId="154"/>
-    <tableColumn id="8" xr3:uid="{80075233-98B6-4069-925B-B0535C380529}" name="Top_Run_Scorer" dataDxfId="153"/>
-    <tableColumn id="9" xr3:uid="{150DCABE-6CB8-4FC1-932F-217514F9A86C}" name="Top_Wicket_Taker" dataDxfId="152"/>
-    <tableColumn id="10" xr3:uid="{05DDC266-2D52-4707-A26B-24A9E0EBBF9A}" name="Emerging_Player" dataDxfId="151"/>
-    <tableColumn id="11" xr3:uid="{31785DAE-EE50-4C9E-ADE5-07EF07C039B3}" name="Key_All_Rounder" dataDxfId="150"/>
+    <tableColumn id="1" xr3:uid="{75EBE216-597C-4C4A-B726-D99C39CCDB60}" name="Gender" dataDxfId="70"/>
+    <tableColumn id="2" xr3:uid="{E9F87583-4B25-409A-B140-DFEC87BF0855}" name="Age_Group" dataDxfId="69"/>
+    <tableColumn id="3" xr3:uid="{6CDA1287-CEC1-4795-8B0F-543D1C880301}" name="Team_of_Interest" dataDxfId="68"/>
+    <tableColumn id="4" xr3:uid="{22AEE1FA-C932-4088-A580-94AB0983CB55}" name="Winner" dataDxfId="67"/>
+    <tableColumn id="5" xr3:uid="{25F583BB-3320-4533-9A51-8C2F9A17EB78}" name="Finalists" dataDxfId="66"/>
+    <tableColumn id="6" xr3:uid="{A2BFDA0E-B228-4DA3-B139-0E06004025ED}" name="Strongest_Batting_Lineup" dataDxfId="65"/>
+    <tableColumn id="7" xr3:uid="{1C2F6CC1-A9AC-4C80-B2B0-CD1FF333E7E1}" name="Strongest_Balling_Attack" dataDxfId="64"/>
+    <tableColumn id="8" xr3:uid="{80075233-98B6-4069-925B-B0535C380529}" name="Top_Run_Scorer" dataDxfId="63"/>
+    <tableColumn id="9" xr3:uid="{150DCABE-6CB8-4FC1-932F-217514F9A86C}" name="Top_Wicket_Taker" dataDxfId="62"/>
+    <tableColumn id="10" xr3:uid="{05DDC266-2D52-4707-A26B-24A9E0EBBF9A}" name="Emerging_Player" dataDxfId="61"/>
+    <tableColumn id="11" xr3:uid="{31785DAE-EE50-4C9E-ADE5-07EF07C039B3}" name="Key_All_Rounder" dataDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -13487,170 +12929,170 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="21" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="14" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="14" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="14" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="14" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="14" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="14" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="14" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="14" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="34.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="18" t="s">
         <v>105</v>
       </c>
     </row>
@@ -13664,7 +13106,7 @@
   <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="I20" sqref="I15:I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -13717,7 +13159,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -13752,7 +13194,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -13787,7 +13229,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -13822,7 +13264,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
@@ -13857,7 +13299,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -13892,7 +13334,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -13927,7 +13369,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
@@ -13962,7 +13404,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
@@ -13997,7 +13439,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -14032,7 +13474,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -14067,7 +13509,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -14102,7 +13544,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -14137,7 +13579,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -14198,7 +13640,7 @@
         <v>24</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>118</v>
@@ -14207,7 +13649,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
@@ -14242,7 +13684,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
@@ -14277,7 +13719,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
@@ -14312,7 +13754,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>26</v>
       </c>
@@ -14382,7 +13824,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
@@ -14417,7 +13859,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>12</v>
       </c>
@@ -14478,7 +13920,7 @@
         <v>24</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>25</v>
@@ -14487,7 +13929,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
@@ -14522,7 +13964,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>12</v>
       </c>
@@ -14557,7 +13999,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>12</v>
       </c>
@@ -14592,7 +14034,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>12</v>
       </c>
@@ -14627,7 +14069,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -14662,7 +14104,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>12</v>
       </c>
@@ -14697,7 +14139,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>12</v>
       </c>
@@ -14732,7 +14174,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>12</v>
       </c>
@@ -14767,7 +14209,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>26</v>
       </c>
@@ -14802,7 +14244,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>26</v>
       </c>
@@ -14837,7 +14279,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>12</v>
       </c>
@@ -14872,7 +14314,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>12</v>
       </c>
@@ -14907,7 +14349,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>12</v>
       </c>
@@ -14942,7 +14384,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>26</v>
       </c>
@@ -14977,7 +14419,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>12</v>
       </c>
@@ -15012,7 +14454,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>26</v>
       </c>
@@ -15047,7 +14489,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>12</v>
       </c>
@@ -15082,7 +14524,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>26</v>
       </c>
@@ -15117,7 +14559,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>12</v>
       </c>
@@ -15152,7 +14594,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>12</v>
       </c>
@@ -15187,7 +14629,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>12</v>
       </c>
@@ -15222,7 +14664,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>26</v>
       </c>
@@ -15257,7 +14699,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>12</v>
       </c>
@@ -15292,7 +14734,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>26</v>
       </c>
@@ -15327,7 +14769,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>26</v>
       </c>
@@ -15362,7 +14804,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>12</v>
       </c>
@@ -15397,7 +14839,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>12</v>
       </c>
@@ -15432,7 +14874,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>12</v>
       </c>
@@ -15467,7 +14909,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="19.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>12</v>
       </c>
@@ -15523,10 +14965,10 @@
     <col min="1" max="1" width="20.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.5546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -15537,7 +14979,7 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G3" s="12">
+      <c r="G3" s="23">
         <v>51</v>
       </c>
     </row>
@@ -15564,7 +15006,7 @@
       <c r="G6" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="23">
         <v>17</v>
       </c>
     </row>
@@ -15575,7 +15017,7 @@
       <c r="G7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="23">
         <v>34</v>
       </c>
     </row>
@@ -15614,7 +15056,7 @@
       <c r="N10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="O10" s="12">
+      <c r="O10" s="23">
         <v>12</v>
       </c>
     </row>
@@ -15625,19 +15067,19 @@
       <c r="G11" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="23">
         <v>16</v>
       </c>
       <c r="J11" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="K11" s="12">
+      <c r="K11" s="23">
         <v>9</v>
       </c>
       <c r="N11" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="O11" s="12">
+      <c r="O11" s="23">
         <v>6</v>
       </c>
     </row>
@@ -15648,19 +15090,19 @@
       <c r="G12" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="23">
         <v>15</v>
       </c>
       <c r="J12" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="K12" s="12">
+      <c r="K12" s="23">
         <v>1</v>
       </c>
       <c r="N12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="O12" s="12">
+      <c r="O12" s="23">
         <v>26</v>
       </c>
     </row>
@@ -15671,19 +15113,19 @@
       <c r="G13" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="23">
         <v>6</v>
       </c>
       <c r="J13" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="K13" s="12">
+      <c r="K13" s="23">
         <v>10</v>
       </c>
       <c r="N13" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="O13" s="12">
+      <c r="O13" s="23">
         <v>2</v>
       </c>
     </row>
@@ -15691,19 +15133,19 @@
       <c r="G14" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H14" s="23">
         <v>3</v>
       </c>
       <c r="J14" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="K14" s="12">
+      <c r="K14" s="23">
         <v>22</v>
       </c>
       <c r="N14" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="O14" s="12">
+      <c r="O14" s="23">
         <v>2</v>
       </c>
     </row>
@@ -15711,19 +15153,19 @@
       <c r="G15" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H15" s="23">
         <v>1</v>
       </c>
       <c r="J15" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="K15" s="12">
+      <c r="K15" s="23">
         <v>3</v>
       </c>
       <c r="N15" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="O15" s="12">
+      <c r="O15" s="23">
         <v>1</v>
       </c>
     </row>
@@ -15731,19 +15173,19 @@
       <c r="G16" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H16" s="23">
         <v>10</v>
       </c>
       <c r="J16" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="K16" s="12">
+      <c r="K16" s="23">
         <v>2</v>
       </c>
       <c r="N16" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="O16" s="12">
+      <c r="O16" s="23">
         <v>2</v>
       </c>
     </row>
@@ -15751,7 +15193,7 @@
       <c r="J17" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="K17" s="12">
+      <c r="K17" s="23">
         <v>2</v>
       </c>
     </row>
@@ -15765,7 +15207,7 @@
       <c r="J18" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="K18" s="12">
+      <c r="K18" s="23">
         <v>2</v>
       </c>
     </row>
@@ -15773,7 +15215,7 @@
       <c r="G19" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H19" s="12">
+      <c r="H19" s="23">
         <v>17</v>
       </c>
     </row>
@@ -15781,7 +15223,7 @@
       <c r="G20" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H20" s="12">
+      <c r="H20" s="23">
         <v>34</v>
       </c>
     </row>
@@ -15797,7 +15239,7 @@
       <c r="J23" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="K23" s="12">
+      <c r="K23" s="23">
         <v>26</v>
       </c>
     </row>
@@ -15805,7 +15247,7 @@
       <c r="J24" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="K24" s="12">
+      <c r="K24" s="23">
         <v>1</v>
       </c>
     </row>
@@ -15813,7 +15255,7 @@
       <c r="J25" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="K25" s="12">
+      <c r="K25" s="23">
         <v>2</v>
       </c>
     </row>
@@ -15821,7 +15263,7 @@
       <c r="J26" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="K26" s="12">
+      <c r="K26" s="23">
         <v>13</v>
       </c>
     </row>
@@ -15829,7 +15271,7 @@
       <c r="J27" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="K27" s="12">
+      <c r="K27" s="23">
         <v>2</v>
       </c>
     </row>
@@ -15837,7 +15279,7 @@
       <c r="J28" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="K28" s="12">
+      <c r="K28" s="23">
         <v>2</v>
       </c>
     </row>
@@ -15845,7 +15287,7 @@
       <c r="J29" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="K29" s="12">
+      <c r="K29" s="23">
         <v>2</v>
       </c>
     </row>
@@ -15853,7 +15295,7 @@
       <c r="J30" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="K30" s="12">
+      <c r="K30" s="23">
         <v>2</v>
       </c>
     </row>
@@ -15861,7 +15303,7 @@
       <c r="J31" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="K31" s="12">
+      <c r="K31" s="23">
         <v>1</v>
       </c>
     </row>
@@ -15878,7 +15320,7 @@
   <dimension ref="B6:B7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P73" sqref="P73"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -15887,12 +15329,12 @@
     <col min="2" max="2" width="31.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:2" ht="54.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="23" t="s">
+    <row r="6" spans="2:2" ht="22.8" x14ac:dyDescent="0.25">
+      <c r="B6" s="22" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="54.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" ht="30.6" x14ac:dyDescent="0.25">
       <c r="B7" s="24">
         <v>51</v>
       </c>

</xml_diff>